<commit_message>
Fix report page; - change name report - remove getRequest for report(it was test)
</commit_message>
<xml_diff>
--- a/src/main/resources/report/template/eventsTemplate.xlsx
+++ b/src/main/resources/report/template/eventsTemplate.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egorsafonov/IdeaProjects/ticketSaleSystems/src/main/resources/report/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaWorkProjects\ticketSaleSystems\src\main\resources\report\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C91428-7799-8A44-9002-CD22CDE6463F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="2500" windowWidth="28800" windowHeight="17500" xr2:uid="{E5243EB7-EEB3-D241-9F79-8205A89BF157}"/>
+    <workbookView xWindow="38400" yWindow="2505" windowWidth="28800" windowHeight="17505"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -61,7 +60,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yy\ h:mm;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -92,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -407,21 +410,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0548239-7868-FA45-852E-A1CEC46A2523}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -442,5 +445,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix-reports: - add header for event-report
</commit_message>
<xml_diff>
--- a/src/main/resources/report/template/eventsTemplate.xlsx
+++ b/src/main/resources/report/template/eventsTemplate.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaWorkProjects\ticketSaleSystems\src\main\resources\report\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egorsafonov/IdeaProjects/ticketSaleSystems/src/main/resources/report/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF685879-577B-CF45-9A14-DF497E259B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="2505" windowWidth="28800" windowHeight="17505"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="EventReport">Лист1!$A$1:$F$1</definedName>
+    <definedName name="EventReport">Лист1!$A$2:$F$2</definedName>
+    <definedName name="header">Лист1!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>${event_date}</t>
   </si>
@@ -55,14 +57,32 @@
   </si>
   <si>
     <t>${order_count}</t>
+  </si>
+  <si>
+    <t>Дата мероприятия</t>
+  </si>
+  <si>
+    <t>Площадка</t>
+  </si>
+  <si>
+    <t>Адресс площадки</t>
+  </si>
+  <si>
+    <t>Кол-во билетов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумма </t>
+  </si>
+  <si>
+    <t>Кол-во заказов</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -96,7 +116,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -410,36 +430,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>